<commit_message>
updated facility location formulation and preliminary flexibility case
</commit_message>
<xml_diff>
--- a/Multiknapsack/summary.xlsx
+++ b/Multiknapsack/summary.xlsx
@@ -8,18 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagan024\Desktop\CCG-RODDU\Multiknapsack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0DCE91-BB55-4011-9711-A128CA6BA623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F909AC0D-C4F9-465E-B01E-69AF99231E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1215" yWindow="2940" windowWidth="21495" windowHeight="11190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed recourse" sheetId="1" r:id="rId1"/>
     <sheet name="random recourse" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -56,6 +67,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,14 +107,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,6 +412,7 @@
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="13" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" dyDescent="0.25" s="1" customFormat="1">
@@ -408,14 +428,14 @@
       <c r="D1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" t="s" s="2">
+      <c r="F1" s="4"/>
+      <c r="G1" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" dyDescent="0.25" s="1" customFormat="1">
       <c r="E2" t="s" s="1">
@@ -444,20 +464,20 @@
       <c r="D3">
         <v>0.25</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>-112.50781279345111</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>-112.50781279345111</v>
       </c>
-      <c r="G3">
-        <v>0.9874096535</v>
-      </c>
-      <c r="H3">
-        <v>0.8253634682999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="G3" s="2">
+        <v>0.98740965349999998</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.82536346829999974</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -470,20 +490,20 @@
       <c r="D4">
         <v>0.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>-214.50399986426677</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>-214.50399986426677</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>1.0468694129</v>
       </c>
-      <c r="H4">
-        <v>0.9928197042000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="2">
+        <v>0.99281970420000021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" dyDescent="0.25">
       <c r="A5">
         <v>20</v>
       </c>
@@ -496,20 +516,20 @@
       <c r="D5">
         <v>0.75</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>-303.80842325610934</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>-303.80842325610934</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>1.0231255444999998</v>
       </c>
-      <c r="H5">
-        <v>0.9100288637</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5" s="2">
+        <v>0.91002886370000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -522,20 +542,20 @@
       <c r="D6">
         <v>0.25</v>
       </c>
-      <c r="E6">
-        <v>-229.2929854006456</v>
-      </c>
-      <c r="F6">
-        <v>-229.2929854006456</v>
-      </c>
-      <c r="G6">
-        <v>2.3250055054</v>
-      </c>
-      <c r="H6">
+      <c r="E6" s="3">
+        <v>-229.29298540064559</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-229.29298540064559</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2.3250055054000001</v>
+      </c>
+      <c r="H6" s="2">
         <v>0.9611292305000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
@@ -548,20 +568,20 @@
       <c r="D7">
         <v>0.5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>-431.08001257734134</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>-431.08001257734134</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>2.5631548166</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>1.0905419657999997</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" dyDescent="0.25">
       <c r="A8">
         <v>20</v>
       </c>
@@ -574,20 +594,20 @@
       <c r="D8">
         <v>0.75</v>
       </c>
-      <c r="E8">
-        <v>-606.1197236677168</v>
-      </c>
-      <c r="F8">
-        <v>-606.1197236677168</v>
-      </c>
-      <c r="G8">
-        <v>2.0988124143</v>
-      </c>
-      <c r="H8">
-        <v>0.8260524738000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="E8" s="3">
+        <v>-606.11972366771681</v>
+      </c>
+      <c r="F8" s="3">
+        <v>-606.11972366771681</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2.0988124143000002</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.82605247380000013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" dyDescent="0.25">
       <c r="A9">
         <v>50</v>
       </c>
@@ -600,20 +620,20 @@
       <c r="D9">
         <v>0.25</v>
       </c>
-      <c r="E9">
-        <v>-824.9585417731884</v>
-      </c>
-      <c r="F9">
-        <v>-824.9585417731884</v>
-      </c>
-      <c r="G9">
+      <c r="E9" s="3">
+        <v>-824.95854177318836</v>
+      </c>
+      <c r="F9" s="3">
+        <v>-824.95854177318836</v>
+      </c>
+      <c r="G9" s="2">
         <v>177.73769103709998</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>1.1653906519000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" dyDescent="0.25">
       <c r="A10">
         <v>50</v>
       </c>
@@ -626,20 +646,20 @@
       <c r="D10">
         <v>0.5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>-1600.1578268991093</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>-1600.1578268991093</v>
       </c>
-      <c r="G10">
-        <v>174.4319925361</v>
-      </c>
-      <c r="H10">
-        <v>0.9988185052999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="G10" s="2">
+        <v>174.43199253610001</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.99881850529999983</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" dyDescent="0.25">
       <c r="A11">
         <v>50</v>
       </c>
@@ -652,20 +672,20 @@
       <c r="D11">
         <v>0.75</v>
       </c>
-      <c r="E11">
-        <v>-2326.130834786616</v>
-      </c>
-      <c r="F11">
-        <v>-2326.130834786616</v>
-      </c>
-      <c r="G11">
+      <c r="E11" s="3">
+        <v>-2326.1308347866161</v>
+      </c>
+      <c r="F11" s="3">
+        <v>-2326.1308347866161</v>
+      </c>
+      <c r="G11" s="2">
         <v>202.6266498164</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>1.0304561054999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" dyDescent="0.25">
       <c r="A12">
         <v>100</v>
       </c>
@@ -678,20 +698,20 @@
       <c r="D12">
         <v>0.25</v>
       </c>
-      <c r="E12">
-        <v>-1430.627565748336</v>
-      </c>
-      <c r="F12">
-        <v>-1430.627565748336</v>
-      </c>
-      <c r="G12">
+      <c r="E12" s="3">
+        <v>-1430.6275657483361</v>
+      </c>
+      <c r="F12" s="3">
+        <v>-1430.6275657483361</v>
+      </c>
+      <c r="G12" s="2">
         <v>2599.5169996945997</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>1.0734798929</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" dyDescent="0.25">
       <c r="A13">
         <v>100</v>
       </c>
@@ -704,20 +724,20 @@
       <c r="D13">
         <v>0.5</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>-2828.002586206353</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>-2828.002586206353</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>2624.3790065872004</v>
       </c>
-      <c r="H13">
-        <v>1.1918019451</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="H13" s="2">
+        <v>1.1918019450999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" dyDescent="0.25">
       <c r="A14">
         <v>100</v>
       </c>
@@ -730,20 +750,20 @@
       <c r="D14">
         <v>0.75</v>
       </c>
-      <c r="E14">
-        <v>-4182.042743391336</v>
-      </c>
-      <c r="F14">
-        <v>-4182.042743391335</v>
-      </c>
-      <c r="G14">
-        <v>2597.769042666</v>
-      </c>
-      <c r="H14">
+      <c r="E14" s="3">
+        <v>-4182.0427433913364</v>
+      </c>
+      <c r="F14" s="3">
+        <v>-4182.0427433913346</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2597.7690426660001</v>
+      </c>
+      <c r="H14" s="2">
         <v>1.1735646413999998</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" dyDescent="0.25">
       <c r="A15">
         <v>200</v>
       </c>
@@ -768,10 +788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001CC449-0275-4E6D-A820-B5F8FE4E947F}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,7 +806,7 @@
     <col min="17" max="17" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" dyDescent="0.25" s="1" customFormat="1">
+    <row r="1" spans="1:18" dyDescent="0.25" s="1" customFormat="1">
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
@@ -799,20 +819,20 @@
       <c r="D1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" t="s" s="2">
+      <c r="F1" s="4"/>
+      <c r="G1" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" dyDescent="0.25">
+      <c r="H1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -837,7 +857,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A3">
         <v>5</v>
       </c>
@@ -850,20 +870,12 @@
       <c r="D3">
         <v>0.25</v>
       </c>
-      <c r="E3">
-        <v>-12.163928218490579</v>
-      </c>
-      <c r="F3">
-        <v>-12.16748247853319</v>
-      </c>
-      <c r="G3">
-        <v>0.40139375610000005</v>
-      </c>
-      <c r="H3">
-        <v>1.2537145891</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A4">
         <v>5</v>
       </c>
@@ -876,20 +888,12 @@
       <c r="D4">
         <v>0.5</v>
       </c>
-      <c r="E4">
-        <v>-21.80335789394766</v>
-      </c>
-      <c r="F4">
-        <v>-21.808523223657478</v>
-      </c>
-      <c r="G4">
-        <v>0.38486517749999993</v>
-      </c>
-      <c r="H4">
-        <v>1.3494863101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A5">
         <v>5</v>
       </c>
@@ -902,400 +906,238 @@
       <c r="D5">
         <v>0.75</v>
       </c>
-      <c r="E5">
-        <v>-29.785902443064664</v>
-      </c>
-      <c r="F5">
-        <v>-29.79751750335372</v>
-      </c>
-      <c r="G5">
-        <v>0.34527888510000004</v>
-      </c>
-      <c r="H5">
-        <v>1.2806085982000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0.25</v>
       </c>
-      <c r="E6">
-        <v>-10.045808862443698</v>
-      </c>
-      <c r="F6">
-        <v>-10.047000068681587</v>
-      </c>
-      <c r="G6">
-        <v>1.6010671378</v>
-      </c>
-      <c r="H6">
-        <v>8.644079874100001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+    </row>
+    <row r="7" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0.5</v>
       </c>
-      <c r="E7">
-        <v>-17.49957856646698</v>
-      </c>
-      <c r="F7">
-        <v>-17.5026695570849</v>
-      </c>
-      <c r="G7">
-        <v>0.6873397005000002</v>
-      </c>
-      <c r="H7">
-        <v>4.4398905965</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+    </row>
+    <row r="8" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0.75</v>
       </c>
-      <c r="E8">
-        <v>-23.456288857076025</v>
-      </c>
-      <c r="F8">
-        <v>-23.461737632657403</v>
-      </c>
-      <c r="G8">
-        <v>0.5140079432</v>
-      </c>
-      <c r="H8">
-        <v>2.0940532508999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0.25</v>
       </c>
-      <c r="E9">
-        <v>-25.63746671688179</v>
-      </c>
-      <c r="F9">
-        <v>-25.644245480216206</v>
-      </c>
-      <c r="G9">
-        <v>0.8542571552</v>
-      </c>
-      <c r="H9">
-        <v>2.6975759091000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+    </row>
+    <row r="10" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>0.5</v>
       </c>
-      <c r="E10">
-        <v>-44.364548903960504</v>
-      </c>
-      <c r="F10">
-        <v>-44.37513181422999</v>
-      </c>
-      <c r="G10">
-        <v>0.5713584864</v>
-      </c>
-      <c r="H10">
-        <v>2.4058158588</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>0.75</v>
       </c>
-      <c r="E11">
-        <v>-58.26136009909508</v>
-      </c>
-      <c r="F11">
-        <v>-58.27800907939186</v>
-      </c>
-      <c r="G11">
-        <v>0.8082877004</v>
-      </c>
-      <c r="H11">
-        <v>2.4508732355</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+    </row>
+    <row r="12" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
       <c r="A12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0.25</v>
       </c>
-      <c r="E12">
-        <v>-22.128452365997692</v>
-      </c>
-      <c r="F12">
-        <v>-22.12974191296592</v>
-      </c>
-      <c r="G12">
-        <v>3065.8359351392996</v>
-      </c>
-      <c r="H12">
-        <v>71.13271126389999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="1:18" dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0.5</v>
       </c>
-      <c r="E13">
-        <v>-37.26936446743676</v>
-      </c>
-      <c r="F13">
-        <v>-37.27209727529485</v>
-      </c>
-      <c r="G13">
-        <v>487.40700586180003</v>
-      </c>
-      <c r="H13">
-        <v>29.0845716004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" dyDescent="0.25">
       <c r="A14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>0.75</v>
       </c>
-      <c r="E14">
-        <v>-48.977631843915844</v>
-      </c>
-      <c r="F14">
-        <v>-48.984342615703106</v>
-      </c>
-      <c r="G14">
-        <v>17.3971972397</v>
-      </c>
-      <c r="H14">
-        <v>12.615008851099999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15">
-        <v>20</v>
-      </c>
-      <c r="B15">
-        <v>40</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <v>0.25</v>
-      </c>
-      <c r="E15">
-        <v>-78.03910142837279</v>
-      </c>
-      <c r="F15">
-        <v>-78.06799711964855</v>
-      </c>
-      <c r="G15">
-        <v>126.57289061649999</v>
-      </c>
-      <c r="H15">
-        <v>3861.4894958815007</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16">
-        <v>20</v>
-      </c>
-      <c r="B16">
-        <v>40</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>0.5</v>
-      </c>
-      <c r="E16">
-        <v>-139.913769532829</v>
-      </c>
-      <c r="F16">
-        <v>-139.9946833122377</v>
-      </c>
-      <c r="G16">
-        <v>47.66611246320001</v>
-      </c>
-      <c r="H16">
-        <v>3533.7267570714002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <v>40</v>
-      </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <v>0.75</v>
-      </c>
-      <c r="E17">
-        <v>-185.68747354904966</v>
-      </c>
-      <c r="F17">
-        <v>-185.72846276564914</v>
-      </c>
-      <c r="G17">
-        <v>51.177189923499995</v>
-      </c>
-      <c r="H17">
-        <v>1609.697828431</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>40</v>
-      </c>
-      <c r="C18">
-        <v>20</v>
-      </c>
-      <c r="D18">
-        <v>0.25</v>
-      </c>
-      <c r="E18">
-        <v>-64.63434406475768</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18">
-        <v>3601.0248421372003</v>
-      </c>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>40</v>
-      </c>
-      <c r="C19">
-        <v>20</v>
-      </c>
-      <c r="D19">
-        <v>0.5</v>
-      </c>
-      <c r="E19"/>
-      <c r="F19">
-        <v>-107.64940952857219</v>
-      </c>
-      <c r="G19"/>
-      <c r="H19">
-        <v>3743.3751806121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>40</v>
-      </c>
-      <c r="C20">
-        <v>20</v>
-      </c>
-      <c r="D20">
-        <v>0.75</v>
-      </c>
-      <c r="E20">
-        <v>-141.30645950043464</v>
-      </c>
-      <c r="F20">
-        <v>-141.34818251478583</v>
-      </c>
-      <c r="G20">
-        <v>174.6022121007</v>
-      </c>
-      <c r="H20">
-        <v>1869.1343710826</v>
-      </c>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" dyDescent="0.25">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" dyDescent="0.25">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="1:18" dyDescent="0.25">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
file cleanup, corrected project toml, working version for MKS and RFL
</commit_message>
<xml_diff>
--- a/Multiknapsack/summary.xlsx
+++ b/Multiknapsack/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagan024\Desktop\CCG-RODDU\Multiknapsack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F909AC0D-C4F9-465E-B01E-69AF99231E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36157A53-710D-4373-BA3A-995C7066FCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="2940" windowWidth="21495" windowHeight="11190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed recourse" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>M</t>
   </si>
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -117,9 +117,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,43 +412,43 @@
     <col min="13" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" dyDescent="0.25" s="1" customFormat="1">
-      <c r="A1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="4">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4"/>
-      <c r="G1" t="s" s="4">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" dyDescent="0.25" s="1" customFormat="1">
-      <c r="E2" t="s" s="1">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="1">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="1">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s" s="1">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -477,7 +474,7 @@
         <v>0.82536346829999974</v>
       </c>
     </row>
-    <row r="4" spans="1:8" dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -503,7 +500,7 @@
         <v>0.99281970420000021</v>
       </c>
     </row>
-    <row r="5" spans="1:8" dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20</v>
       </c>
@@ -529,7 +526,7 @@
         <v>0.91002886370000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -555,7 +552,7 @@
         <v>0.9611292305000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
@@ -581,7 +578,7 @@
         <v>1.0905419657999997</v>
       </c>
     </row>
-    <row r="8" spans="1:8" dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20</v>
       </c>
@@ -607,7 +604,7 @@
         <v>0.82605247380000013</v>
       </c>
     </row>
-    <row r="9" spans="1:8" dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>50</v>
       </c>
@@ -633,7 +630,7 @@
         <v>1.1653906519000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>50</v>
       </c>
@@ -659,7 +656,7 @@
         <v>0.99881850529999983</v>
       </c>
     </row>
-    <row r="11" spans="1:8" dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>50</v>
       </c>
@@ -685,7 +682,7 @@
         <v>1.0304561054999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8" dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100</v>
       </c>
@@ -711,7 +708,7 @@
         <v>1.0734798929</v>
       </c>
     </row>
-    <row r="13" spans="1:8" dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>100</v>
       </c>
@@ -737,7 +734,7 @@
         <v>1.1918019450999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>100</v>
       </c>
@@ -761,20 +758,6 @@
       </c>
       <c r="H14" s="2">
         <v>1.1735646413999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" dyDescent="0.25">
-      <c r="A15">
-        <v>200</v>
-      </c>
-      <c r="B15">
-        <v>400</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -790,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001CC449-0275-4E6D-A820-B5F8FE4E947F}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -806,24 +789,24 @@
     <col min="17" max="17" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" dyDescent="0.25" s="1" customFormat="1">
-      <c r="A1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="1">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="4">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4"/>
-      <c r="G1" t="s" s="4">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4"/>
@@ -832,21 +815,21 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:18" dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" t="s" s="1">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="1">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="1">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s" s="1">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="1"/>
@@ -857,7 +840,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -870,12 +853,8 @@
       <c r="D3">
         <v>0.25</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -888,12 +867,8 @@
       <c r="D4">
         <v>0.5</v>
       </c>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -906,12 +881,8 @@
       <c r="D5">
         <v>0.75</v>
       </c>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -924,16 +895,12 @@
       <c r="D6">
         <v>0.25</v>
       </c>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-    </row>
-    <row r="7" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -946,16 +913,12 @@
       <c r="D7">
         <v>0.5</v>
       </c>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-    </row>
-    <row r="8" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -968,16 +931,12 @@
       <c r="D8">
         <v>0.75</v>
       </c>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-    </row>
-    <row r="9" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -990,16 +949,12 @@
       <c r="D9">
         <v>0.25</v>
       </c>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-    </row>
-    <row r="10" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1012,16 +967,12 @@
       <c r="D10">
         <v>0.5</v>
       </c>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-    </row>
-    <row r="11" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1034,16 +985,12 @@
       <c r="D11">
         <v>0.75</v>
       </c>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-    </row>
-    <row r="12" spans="1:18" dyDescent="0.25" s="5" customFormat="1">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20</v>
       </c>
@@ -1056,16 +1003,12 @@
       <c r="D12">
         <v>0.25</v>
       </c>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-    </row>
-    <row r="13" spans="1:18" dyDescent="0.25">
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20</v>
       </c>
@@ -1078,16 +1021,12 @@
       <c r="D13">
         <v>0.5</v>
       </c>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20</v>
       </c>
@@ -1100,16 +1039,12 @@
       <c r="D14">
         <v>0.75</v>
       </c>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="2"/>
@@ -1119,7 +1054,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="2"/>
@@ -1129,7 +1064,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" dyDescent="0.25">
+    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="2"/>

</xml_diff>